<commit_message>
Update USMC Example (Optimization).xlsx
</commit_message>
<xml_diff>
--- a/MS Excel Examples/USMC Example (Optimization).xlsx
+++ b/MS Excel Examples/USMC Example (Optimization).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roque\OneDrive\Desktop\CANA\IRAD Courses\Veterans Course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roque\OneDrive\Documents\GitHub\Training-Resources\MS Excel Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41573FBB-B9B4-439F-B5CA-2EE3601E53D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9410F0B-9E1E-4DD1-9E98-70186A1A4C93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{53C7F6D1-1AF4-4379-9A69-13EF41661E03}"/>
   </bookViews>
@@ -23,31 +23,37 @@
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$5</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$E$10</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$E$11</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$E$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$5</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$C$5</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$E$10</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$E$11</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Sheet1!$E$9</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">7</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$E$5</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$F$10</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$F$11</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$F$9</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$F$10</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Sheet1!$F$11</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Sheet1!$F$9</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -379,6 +385,187 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93CD2EBD-6193-4807-82BB-A54BAF2D8633}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6453187" y="1457325"/>
+          <a:ext cx="2052638" cy="295277"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>323852</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F66FDD6-2B1D-46A1-B3B2-07DBFF40B9C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6453188" y="1776413"/>
+          <a:ext cx="2052638" cy="276227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9527</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E72ADF79-53D0-4F24-8E5E-31ED4C578BA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6457949" y="2095500"/>
+          <a:ext cx="2066925" cy="266702"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>33338</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>608302</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D71553-5125-401F-B2C7-D6F3B7E2235A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5815013" y="647698"/>
+          <a:ext cx="1870364" cy="342901"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -681,7 +868,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -727,15 +914,15 @@
         <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>122.00000000000001</v>
+        <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>77.999999999999986</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="3">
         <f>($B$5*$B$6)+($C$5*$C$6)</f>
-        <v>66100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -762,7 +949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -774,13 +961,13 @@
       </c>
       <c r="E9">
         <f>($B9*$B$5)+($C9*$C$5)</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -792,13 +979,13 @@
       </c>
       <c r="E10">
         <f>($B10*$B$5)+($C10*$C$5)</f>
-        <v>1566</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>1566</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -810,7 +997,7 @@
       </c>
       <c r="E11">
         <f>($B11*$B$5)+($C11*$C$5)</f>
-        <v>2712</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>2880</v>
@@ -829,6 +1016,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>